<commit_message>
use case interpretar comando melhorado
</commit_message>
<xml_diff>
--- a/use-cases/use-case-interpretar-comando-de-voz.xlsx
+++ b/use-cases/use-case-interpretar-comando-de-voz.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopetronilho/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopetronilho/Desktop/LI 4/li4-project/use-cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B34395-852D-7B45-923C-AD17A8316812}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45560A72-D9E2-A14A-81A2-FE564DF6BBC3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Actor input</t>
   </si>
@@ -33,10 +33,6 @@
     <t>System response</t>
   </si>
   <si>
-    <t>Cenário 
-Normal</t>
-  </si>
-  <si>
     <t>Use Case:</t>
   </si>
   <si>
@@ -52,102 +48,268 @@
     <t>Utilizador</t>
   </si>
   <si>
-    <t>Estar autenticado no sistema</t>
-  </si>
-  <si>
-    <t>4.3. o processo é terminado.</t>
-  </si>
-  <si>
     <t>Interpretar o comando de voz</t>
   </si>
   <si>
-    <t>Interpretou o comando de voz com sucesso</t>
-  </si>
-  <si>
-    <t>1. ator diz comando de voz.</t>
-  </si>
-  <si>
-    <t>2. sistema interpreta comando de voz.</t>
-  </si>
-  <si>
-    <t>Alternativa 6
-[sistema não reconheceu o comando de voz]
-(passo 2)</t>
-  </si>
-  <si>
-    <t>Alternativa 1
-[comando reconhecido é "Go Next"]
-(passo 2)</t>
-  </si>
-  <si>
-    <t>1.1. o passo seguinte é apresentado no ecrã.</t>
-  </si>
-  <si>
-    <t>1.2. o passo seguinte é ditado em voz alta.</t>
-  </si>
-  <si>
-    <t>1.3. o processo é terminado.</t>
-  </si>
-  <si>
-    <t>Alternativa 2
-[comando reconhecido é "Go Back"]
-(passo 2)</t>
-  </si>
-  <si>
-    <t>2.1. o passo anteior é apresentado no ecrã.</t>
-  </si>
-  <si>
-    <t>2.2. o passo anterior é ditado em voz alta.</t>
-  </si>
-  <si>
-    <t>2.3. o processo é terminado.</t>
-  </si>
-  <si>
-    <t>Alternativa 3
+    <t>6.1. sistema informa que não reconheceu o
+ comando de voz.</t>
+  </si>
+  <si>
+    <t>2. ator diz "Hey Cheli".</t>
+  </si>
+  <si>
+    <t>4. sistema escuta próximo comando de voz.</t>
+  </si>
+  <si>
+    <t>1. sistema está à escuta de uma expressão.</t>
+  </si>
+  <si>
+    <t>3. sistema valida expressão escutada verificando se corresponde à expressão "Hey Cheli".</t>
+  </si>
+  <si>
+    <t>5. ator diz comando de voz.</t>
+  </si>
+  <si>
+    <t>6. sistema interpreta comando de voz.</t>
+  </si>
+  <si>
+    <t>Alternativa 4
 [comando reconhecido é "Repeat"]
-(passo 2)</t>
-  </si>
-  <si>
-    <t>3.1. o passo atual é ditado em voz alta.</t>
-  </si>
-  <si>
-    <t>3.2. o processo é terminado.</t>
-  </si>
-  <si>
-    <t>Alternativa 4
+(passo 6)</t>
+  </si>
+  <si>
+    <t>Alternativa 5
 [comando reconhecido é "Help"]
 (passo 2)</t>
   </si>
   <si>
-    <t>4.1. o primeiro passo é apresentado no ecrã.</t>
-  </si>
-  <si>
-    <t>4.2. o primeiro passo é ditado em voz alta.</t>
-  </si>
-  <si>
-    <t>6.2. o processo é terminado.</t>
-  </si>
-  <si>
-    <t>6.1. sistema informa que não reconheceu o
- comando de voz.</t>
-  </si>
-  <si>
-    <t>Alternativa 5
+    <t>Alternativa 6
 [ator encontra-se no passo 1 e comando reconhecido é "Start"]
-(passo 2)</t>
-  </si>
-  <si>
-    <t>4.1. é apresentada a lista de comandos por voz.</t>
-  </si>
-  <si>
-    <t>4.2. a lista de comandos por voz é ditada em voz alta.</t>
+(passo 6)</t>
+  </si>
+  <si>
+    <t>6.1. o primeiro passo é apresentado no ecrã.</t>
+  </si>
+  <si>
+    <t>6.2. o primeiro passo é ditado em voz alta.</t>
+  </si>
+  <si>
+    <t>6.3.  regressa ao passo 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Alternativa 7
+[comando reconhecido é "Tell me expressions"]
+(passo 6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Cenário 
+Normal</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Alternativa 3
+[ator </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>não</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> se encontra no passo 1 e comando reconhecido é "Go Back"]
+(passo 6)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Alternativa 2
+[ator </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>não</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> se encontra no último passo e comando reconhecido é "Go Next"]
+(passo 6)</t>
+    </r>
+  </si>
+  <si>
+    <t>3.1. regressa ao passo 1.</t>
+  </si>
+  <si>
+    <t>6.1. o passo seguinte é apresentado no ecrã.</t>
+  </si>
+  <si>
+    <t>6.2. o passo seguinte é ditado em voz alta.</t>
+  </si>
+  <si>
+    <t>6.1. o passo anteior é apresentado no ecrã.</t>
+  </si>
+  <si>
+    <t>6.2. o passo anterior é ditado em voz alta.</t>
+  </si>
+  <si>
+    <t>6.1. o passo atual é ditado em voz alta.</t>
+  </si>
+  <si>
+    <t>6.2.  regressa ao passo 1.</t>
+  </si>
+  <si>
+    <t>6.1. é apresentada a lista de comandos por voz.</t>
+  </si>
+  <si>
+    <t>6.2. a lista de comandos por voz é ditada em voz alta.</t>
+  </si>
+  <si>
+    <t>6.1. sistema diz:
+ "From the following expressions point me the number which you did not understand: 
+1 - ...
+2 - ...
+N - ...".</t>
+  </si>
+  <si>
+    <t>6.2. sistema fica à escuta do número da expressão.</t>
+  </si>
+  <si>
+    <t>6.3. ator diz o número da expressão.</t>
+  </si>
+  <si>
+    <t>6.4. sistema interpreta ditado do utilizador verificando se corresponde a um número (e caso seja, se corresponde a uma expressão).</t>
+  </si>
+  <si>
+    <t>6.5. &lt;&lt;include&gt;&gt; pesquisa expressão</t>
+  </si>
+  <si>
+    <t>6.6.  regressa ao passo 1.</t>
+  </si>
+  <si>
+    <t>6.4.2.  regressa ao passo 1.</t>
+  </si>
+  <si>
+    <t>6.4.1. sistema informa que não reconheceu o
+ a expressão ditada.</t>
+  </si>
+  <si>
+    <t>Ator está autenticado no sistema</t>
+  </si>
+  <si>
+    <t>Interpretou o comando de voz</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Alternativa 1
+[expressão </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>não</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> corresponde a "Hey Cheli"]
+(passo 3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Alternativa 7.1
+[sistema </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>não</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> reconheceu o número da expressão]
+(passo 6.4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Alternativa 8
+[sistema </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>não</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> reconheceu o comando de voz]
+(passo 6)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -161,6 +323,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="3">
@@ -177,7 +346,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -385,11 +554,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -401,36 +631,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -440,17 +660,60 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -767,60 +1030,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
-  <dimension ref="B1:E25"/>
+  <dimension ref="B1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="37.1640625" customWidth="1"/>
+    <col min="2" max="2" width="51.6640625" customWidth="1"/>
     <col min="3" max="3" width="44.6640625" customWidth="1"/>
     <col min="4" max="4" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="17" thickBot="1"/>
+    <row r="2" spans="2:4" ht="20" thickBot="1">
       <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="2:4" ht="20" thickBot="1">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="9"/>
-    </row>
-    <row r="3" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="2:4" ht="20" thickBot="1">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="2:4" ht="20" thickBot="1">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="11"/>
-    </row>
-    <row r="6" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
-        <v>2</v>
+      <c r="C5" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="2:4" ht="20" thickBot="1">
+      <c r="B6" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>0</v>
@@ -829,161 +1092,256 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
-      <c r="C7" s="3" t="s">
+    <row r="7" spans="2:4" ht="20" thickBot="1">
+      <c r="B7" s="22"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="20" thickBot="1">
+      <c r="B8" s="23"/>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="41" thickBot="1">
+      <c r="B9" s="23"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="18" t="s">
+    </row>
+    <row r="10" spans="2:4" ht="25" customHeight="1" thickBot="1">
+      <c r="B10" s="23"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="20" thickBot="1">
+      <c r="B11" s="23"/>
+      <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="7"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="1" t="s">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="20" thickBot="1">
+      <c r="B12" s="23"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" s="32" customFormat="1" ht="86" customHeight="1" thickBot="1">
+      <c r="B13" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="31"/>
+      <c r="D13" s="33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="29" customHeight="1" thickBot="1">
+      <c r="B14" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="26" customHeight="1" thickBot="1">
+      <c r="B15" s="14"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="29" customHeight="1" thickBot="1">
+      <c r="B16" s="14"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14" t="s">
+    <row r="17" spans="2:4" ht="27" customHeight="1" thickBot="1">
+      <c r="B17" s="13" t="s">
         <v>23</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="7"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="s">
-        <v>26</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="20" x14ac:dyDescent="0.25">
-      <c r="B18" s="20"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="27" customHeight="1" thickBot="1">
+      <c r="B18" s="14"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="21"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="B20" s="19" t="s">
-        <v>31</v>
+      <c r="D18" s="34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="27" customHeight="1" thickBot="1">
+      <c r="B19" s="14"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="29" customHeight="1" thickBot="1">
+      <c r="B20" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="47" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="20"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="21"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="62" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="D25" s="22"/>
-      <c r="E25" s="23"/>
+    <row r="21" spans="2:4" ht="31" customHeight="1" thickBot="1">
+      <c r="B21" s="14"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="19">
+      <c r="B22" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="26" customHeight="1">
+      <c r="B23" s="16"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="20" thickBot="1">
+      <c r="B24" s="17"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="33" customHeight="1">
+      <c r="B25" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="33" customHeight="1">
+      <c r="B26" s="16"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="24" customHeight="1" thickBot="1">
+      <c r="B27" s="17"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="128" customHeight="1" thickBot="1">
+      <c r="B28" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="37" customHeight="1" thickBot="1">
+      <c r="B29" s="13"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="35" customHeight="1" thickBot="1">
+      <c r="B30" s="13"/>
+      <c r="C30" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="35"/>
+    </row>
+    <row r="31" spans="2:4" ht="68" customHeight="1" thickBot="1">
+      <c r="B31" s="13"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="43" customHeight="1" thickBot="1">
+      <c r="B32" s="13"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="39" customHeight="1" thickBot="1">
+      <c r="B33" s="13"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="40">
+      <c r="B34" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="42" customHeight="1" thickBot="1">
+      <c r="B35" s="17"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="40">
+      <c r="B36" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="27" customHeight="1" thickBot="1">
+      <c r="B37" s="17"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="28" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B9:B11"/>
+  <mergeCells count="13">
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B6:B12"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B28:B33"/>
+    <mergeCell ref="B25:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
interpretar comando de voz feito
</commit_message>
<xml_diff>
--- a/use-cases/use-case-interpretar-comando-de-voz.xlsx
+++ b/use-cases/use-case-interpretar-comando-de-voz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopetronilho/Desktop/LI 4/li4-project/use-cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45560A72-D9E2-A14A-81A2-FE564DF6BBC3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC50EEEF-AF60-994E-92E5-18952010CD5E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,11 +83,6 @@
 (passo 2)</t>
   </si>
   <si>
-    <t>Alternativa 6
-[ator encontra-se no passo 1 e comando reconhecido é "Start"]
-(passo 6)</t>
-  </si>
-  <si>
     <t>6.1. o primeiro passo é apresentado no ecrã.</t>
   </si>
   <si>
@@ -303,6 +298,11 @@
       <t xml:space="preserve"> reconheceu o comando de voz]
 (passo 6)</t>
     </r>
+  </si>
+  <si>
+    <t>Alternativa 6
+[ator encontra-se na introdução da receita - passo 0 -  e comando reconhecido é "Start"]
+(passo 6)</t>
   </si>
 </sst>
 </file>
@@ -645,39 +645,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -715,6 +682,39 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1032,14 +1032,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
   <dimension ref="B1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="51.6640625" customWidth="1"/>
+    <col min="2" max="2" width="53.1640625" customWidth="1"/>
     <col min="3" max="3" width="44.6640625" customWidth="1"/>
     <col min="4" max="4" width="61" customWidth="1"/>
   </cols>
@@ -1049,41 +1049,41 @@
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="19"/>
+      <c r="D2" s="32"/>
     </row>
     <row r="3" spans="2:4" ht="20" thickBot="1">
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="19"/>
+      <c r="D3" s="32"/>
     </row>
     <row r="4" spans="2:4" ht="20" thickBot="1">
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="19"/>
+      <c r="C4" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="32"/>
     </row>
     <row r="5" spans="2:4" ht="20" thickBot="1">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="21"/>
+      <c r="C5" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="34"/>
     </row>
     <row r="6" spans="2:4" ht="20" thickBot="1">
-      <c r="B6" s="22" t="s">
-        <v>22</v>
+      <c r="B6" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>0</v>
@@ -1093,227 +1093,227 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="20" thickBot="1">
-      <c r="B7" s="22"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25" t="s">
+      <c r="B7" s="35"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="20" thickBot="1">
-      <c r="B8" s="23"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="41" thickBot="1">
-      <c r="B9" s="23"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="3"/>
       <c r="D9" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="25" customHeight="1" thickBot="1">
-      <c r="B10" s="23"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="3"/>
       <c r="D10" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="20" thickBot="1">
-      <c r="B11" s="23"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="20" thickBot="1">
-      <c r="B12" s="23"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="29" t="s">
+      <c r="B12" s="36"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:4" s="32" customFormat="1" ht="86" customHeight="1" thickBot="1">
-      <c r="B13" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="33" t="s">
-        <v>25</v>
+    <row r="13" spans="2:4" s="21" customFormat="1" ht="86" customHeight="1" thickBot="1">
+      <c r="B13" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="22" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="29" customHeight="1" thickBot="1">
-      <c r="B14" s="13" t="s">
-        <v>24</v>
+      <c r="B14" s="29" t="s">
+        <v>23</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="26" customHeight="1" thickBot="1">
-      <c r="B15" s="14"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="3"/>
       <c r="D15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="29" customHeight="1" thickBot="1">
-      <c r="B16" s="14"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="7"/>
       <c r="D16" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="27" customHeight="1" thickBot="1">
-      <c r="B17" s="13" t="s">
-        <v>23</v>
+      <c r="B17" s="29" t="s">
+        <v>22</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="27" customHeight="1" thickBot="1">
+      <c r="B18" s="30"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="27" customHeight="1" thickBot="1">
-      <c r="B18" s="14"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="34" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="19" spans="2:4" ht="27" customHeight="1" thickBot="1">
-      <c r="B19" s="14"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="7"/>
       <c r="D19" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="29" customHeight="1" thickBot="1">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="29" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="31" customHeight="1" thickBot="1">
-      <c r="B21" s="14"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="7"/>
       <c r="D21" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="19">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="26" customHeight="1">
+      <c r="B23" s="37"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="26" customHeight="1">
-      <c r="B23" s="16"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="27" t="s">
-        <v>33</v>
-      </c>
-    </row>
     <row r="24" spans="2:4" ht="20" thickBot="1">
-      <c r="B24" s="17"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="7"/>
       <c r="D24" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="33" customHeight="1">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="34" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="26" spans="2:4" ht="33" customHeight="1">
-      <c r="B26" s="16"/>
+      <c r="B26" s="37"/>
       <c r="C26" s="3"/>
       <c r="D26" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="24" customHeight="1" thickBot="1">
-      <c r="B27" s="17"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="7"/>
       <c r="D27" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="128" customHeight="1" thickBot="1">
+      <c r="B28" s="29" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" ht="128" customHeight="1" thickBot="1">
-      <c r="B28" s="13" t="s">
-        <v>21</v>
-      </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="36" t="s">
+      <c r="D28" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="37" customHeight="1" thickBot="1">
+      <c r="B29" s="29"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="37" customHeight="1" thickBot="1">
-      <c r="B29" s="13"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="35" t="s">
+    <row r="30" spans="2:4" ht="35" customHeight="1" thickBot="1">
+      <c r="B30" s="29"/>
+      <c r="C30" s="26" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" ht="35" customHeight="1" thickBot="1">
-      <c r="B30" s="13"/>
-      <c r="C30" s="37" t="s">
+      <c r="D30" s="24"/>
+    </row>
+    <row r="31" spans="2:4" ht="68" customHeight="1" thickBot="1">
+      <c r="B31" s="29"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="35"/>
-    </row>
-    <row r="31" spans="2:4" ht="68" customHeight="1" thickBot="1">
-      <c r="B31" s="13"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="35" t="s">
+    </row>
+    <row r="32" spans="2:4" ht="43" customHeight="1" thickBot="1">
+      <c r="B32" s="29"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="43" customHeight="1" thickBot="1">
-      <c r="B32" s="13"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="35" t="s">
+    <row r="33" spans="2:4" ht="39" customHeight="1" thickBot="1">
+      <c r="B33" s="29"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="39" customHeight="1" thickBot="1">
-      <c r="B33" s="13"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="28" t="s">
-        <v>39</v>
-      </c>
-    </row>
     <row r="34" spans="2:4" ht="40">
-      <c r="B34" s="15" t="s">
-        <v>45</v>
+      <c r="B34" s="27" t="s">
+        <v>44</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="42" customHeight="1" thickBot="1">
-      <c r="B35" s="17"/>
+      <c r="B35" s="28"/>
       <c r="C35" s="7"/>
-      <c r="D35" s="28" t="s">
-        <v>40</v>
+      <c r="D35" s="17" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="40">
-      <c r="B36" s="15" t="s">
-        <v>46</v>
+      <c r="B36" s="27" t="s">
+        <v>45</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="10" t="s">
@@ -1321,10 +1321,10 @@
       </c>
     </row>
     <row r="37" spans="2:4" ht="27" customHeight="1" thickBot="1">
-      <c r="B37" s="17"/>
+      <c r="B37" s="28"/>
       <c r="C37" s="7"/>
-      <c r="D37" s="28" t="s">
-        <v>31</v>
+      <c r="D37" s="17" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrigi um erro no diagrama de use case, interpretar-comando-de-voz
</commit_message>
<xml_diff>
--- a/use-cases/use-case-interpretar-comando-de-voz.xlsx
+++ b/use-cases/use-case-interpretar-comando-de-voz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3A2S\LI4\projeto-li4\use-cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josepereira/src/univ/programs/projects/projeto-li4/use-cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C809C9-81FB-4929-8173-80FA722CEAE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5E1F87-0B7D-5045-A815-3EA0C45E081B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="15945" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Actor input</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>6.4. sistema interpreta ditado do utilizador verificando se corresponde a um número (e caso seja, se corresponde a uma expressão).</t>
-  </si>
-  <si>
-    <t>6.5. &lt;&lt;include&gt;&gt; pesquisa expressão</t>
   </si>
   <si>
     <t>6.4.1. sistema informa que não reconheceu o
@@ -267,9 +264,6 @@
     </r>
   </si>
   <si>
-    <t>6.6.  Encerra processo.</t>
-  </si>
-  <si>
     <t>6.4.2.  Encerra processo.</t>
   </si>
   <si>
@@ -303,6 +297,18 @@
     <t>Alternativa 5
 [ator encontra-se na seleção da receita - passo 0 -  e comando reconhecido é "Start"]
 (passo 6)</t>
+  </si>
+  <si>
+    <t>6.5. Recolher a explicação para a expressão.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.6. Apresenta no ecrã a explicação. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.7. Dita a explicação da expressão. </t>
+  </si>
+  <si>
+    <t>6.8.  Encerra processo.</t>
   </si>
 </sst>
 </file>
@@ -734,7 +740,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1030,22 +1036,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
-  <dimension ref="B1:D37"/>
+  <dimension ref="B1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="53.125" customWidth="1"/>
-    <col min="3" max="3" width="44.625" customWidth="1"/>
+    <col min="2" max="2" width="53.1640625" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" customWidth="1"/>
     <col min="4" max="4" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="16.5" thickBot="1"/>
-    <row r="2" spans="2:4" ht="19.5" thickBot="1">
+    <row r="1" spans="2:4" ht="17" thickBot="1"/>
+    <row r="2" spans="2:4" ht="20" thickBot="1">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1054,34 +1060,34 @@
       </c>
       <c r="D2" s="32"/>
     </row>
-    <row r="3" spans="2:4" ht="19.5" thickBot="1">
+    <row r="3" spans="2:4" ht="20" thickBot="1">
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="32"/>
     </row>
-    <row r="4" spans="2:4" ht="19.5" thickBot="1">
+    <row r="4" spans="2:4" ht="20" thickBot="1">
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="32"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" thickBot="1">
+    <row r="5" spans="2:4" ht="20" thickBot="1">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="34"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" thickBot="1">
+    <row r="6" spans="2:4" ht="20" thickBot="1">
       <c r="B6" s="35" t="s">
         <v>16</v>
       </c>
@@ -1092,83 +1098,83 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="19.5" thickBot="1">
+    <row r="7" spans="2:4" ht="20" thickBot="1">
       <c r="B7" s="35"/>
       <c r="C7" s="13"/>
       <c r="D7" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="19.5" thickBot="1">
+    <row r="8" spans="2:4" ht="20" thickBot="1">
       <c r="B8" s="36"/>
       <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="2:4" ht="38.25" thickBot="1">
+    <row r="9" spans="2:4" ht="41" thickBot="1">
       <c r="B9" s="36"/>
       <c r="C9" s="3"/>
       <c r="D9" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="24.95" customHeight="1" thickBot="1">
+    <row r="10" spans="2:4" ht="25" customHeight="1" thickBot="1">
       <c r="B10" s="36"/>
       <c r="C10" s="3"/>
       <c r="D10" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="19.5" thickBot="1">
+    <row r="11" spans="2:4" ht="20" thickBot="1">
       <c r="B11" s="36"/>
       <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:4" ht="19.5" thickBot="1">
+    <row r="12" spans="2:4" ht="20" thickBot="1">
       <c r="B12" s="36"/>
       <c r="C12" s="15"/>
       <c r="D12" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:4" s="21" customFormat="1" ht="86.1" customHeight="1" thickBot="1">
+    <row r="13" spans="2:4" s="21" customFormat="1" ht="86" customHeight="1" thickBot="1">
       <c r="B13" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="29.1" customHeight="1" thickBot="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="29" customHeight="1" thickBot="1">
       <c r="B14" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="26.1" customHeight="1" thickBot="1">
+    <row r="15" spans="2:4" ht="26" customHeight="1" thickBot="1">
       <c r="B15" s="30"/>
       <c r="C15" s="3"/>
       <c r="D15" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="29.1" customHeight="1" thickBot="1">
+    <row r="16" spans="2:4" ht="29" customHeight="1" thickBot="1">
       <c r="B16" s="30"/>
       <c r="C16" s="7"/>
       <c r="D16" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="27" customHeight="1" thickBot="1">
       <c r="B17" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="1" t="s">
@@ -1186,51 +1192,51 @@
       <c r="B19" s="30"/>
       <c r="C19" s="7"/>
       <c r="D19" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="29.1" customHeight="1" thickBot="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="29" customHeight="1" thickBot="1">
       <c r="B20" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="30.95" customHeight="1" thickBot="1">
+    <row r="21" spans="2:4" ht="31" customHeight="1" thickBot="1">
       <c r="B21" s="30"/>
       <c r="C21" s="7"/>
       <c r="D21" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="18.75">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="19">
       <c r="B22" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="26.1" customHeight="1">
+    <row r="23" spans="2:4" ht="26" customHeight="1">
       <c r="B23" s="37"/>
       <c r="C23" s="3"/>
       <c r="D23" s="16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="19.5" thickBot="1">
+    <row r="24" spans="2:4" ht="20" thickBot="1">
       <c r="B24" s="28"/>
       <c r="C24" s="7"/>
       <c r="D24" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="33" customHeight="1">
       <c r="B25" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="23" t="s">
@@ -1248,89 +1254,103 @@
       <c r="B27" s="28"/>
       <c r="C27" s="7"/>
       <c r="D27" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" ht="128.1" customHeight="1" thickBot="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="128" customHeight="1" thickBot="1">
       <c r="B28" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="36.950000000000003" customHeight="1" thickBot="1">
+    <row r="29" spans="2:4" ht="37" customHeight="1" thickBot="1">
       <c r="B29" s="29"/>
       <c r="C29" s="15"/>
       <c r="D29" s="24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="35.1" customHeight="1" thickBot="1">
+    <row r="30" spans="2:4" ht="35" customHeight="1" thickBot="1">
       <c r="B30" s="29"/>
       <c r="C30" s="26" t="s">
         <v>26</v>
       </c>
       <c r="D30" s="24"/>
     </row>
-    <row r="31" spans="2:4" ht="68.099999999999994" customHeight="1" thickBot="1">
+    <row r="31" spans="2:4" ht="68" customHeight="1" thickBot="1">
       <c r="B31" s="29"/>
       <c r="C31" s="26"/>
       <c r="D31" s="24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="42.95" customHeight="1" thickBot="1">
+    <row r="32" spans="2:4" ht="26" customHeight="1" thickBot="1">
       <c r="B32" s="29"/>
-      <c r="C32" s="15"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="39" customHeight="1" thickBot="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="22" customHeight="1" thickBot="1">
       <c r="B33" s="29"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" ht="37.5">
-      <c r="B34" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="42" customHeight="1" thickBot="1">
-      <c r="B35" s="28"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="20" customHeight="1" thickBot="1">
+      <c r="B34" s="29"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="21" customHeight="1" thickBot="1">
+      <c r="B35" s="29"/>
       <c r="C35" s="7"/>
       <c r="D35" s="17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="37.5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="40">
       <c r="B36" s="27" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="27" customHeight="1" thickBot="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="42" customHeight="1" thickBot="1">
       <c r="B37" s="28"/>
       <c r="C37" s="7"/>
       <c r="D37" s="17" t="s">
-        <v>38</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="40">
+      <c r="B38" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="27" customHeight="1" thickBot="1">
+      <c r="B39" s="28"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="17" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B38:B39"/>
     <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B34:B35"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
@@ -1340,7 +1360,7 @@
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B28:B33"/>
+    <mergeCell ref="B28:B35"/>
     <mergeCell ref="B25:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>